<commit_message>
opmized the schedule completer
</commit_message>
<xml_diff>
--- a/SchoolManager/bin/Release/netcoreapp3.1/programa1.xlsx
+++ b/SchoolManager/bin/Release/netcoreapp3.1/programa1.xlsx
@@ -307,72 +307,75 @@
     <t>29</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>14</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>41</t>
+    <t>26</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>26</t>
+    <t>42</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
@@ -382,16 +385,13 @@
     <t>47</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>44</t>
   </si>
   <si>
+    <t>46</t>
+  </si>
+  <si>
     <t>40</t>
-  </si>
-  <si>
-    <t>46</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1785,18 +1785,16 @@
       <c r="N10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1" t="s">
@@ -1810,7 +1808,7 @@
       </c>
       <c r="X10" s="1"/>
       <c r="Y10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Z10" s="1" t="s">
         <v>62</v>
@@ -1819,12 +1817,10 @@
         <v>90</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AC10" s="1"/>
-      <c r="AD10" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="AD10" s="1"/>
       <c r="AE10" s="1" t="s">
         <v>96</v>
       </c>
@@ -1856,7 +1852,9 @@
         <v>75</v>
       </c>
       <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
+      <c r="AR10" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="AS10" s="1" t="s">
         <v>97</v>
       </c>
@@ -1865,9 +1863,11 @@
         <v>94</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW10" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="AX10" s="1"/>
       <c r="AY10" s="1"/>
       <c r="AZ10" s="1"/>
@@ -1881,49 +1881,51 @@
         <v>79</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="U11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="W11" s="1" t="s">
         <v>71</v>
       </c>
@@ -1938,12 +1940,10 @@
         <v>90</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="AD11" s="1"/>
       <c r="AE11" s="1" t="s">
         <v>96</v>
       </c>
@@ -1972,10 +1972,10 @@
       <c r="AP11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AQ11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="AS11" s="1" t="s">
         <v>97</v>
       </c>
@@ -1984,9 +1984,11 @@
         <v>94</v>
       </c>
       <c r="AV11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW11" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="AW11" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="AX11" s="1"/>
       <c r="AY11" s="1"/>
       <c r="AZ11" s="1"/>
@@ -1997,16 +1999,14 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>54</v>
@@ -2019,48 +2019,48 @@
         <v>56</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="L12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P12" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>67</v>
@@ -2068,24 +2068,28 @@
       <c r="AA12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB12" s="1"/>
+      <c r="AB12" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1" t="s">
         <v>99</v>
       </c>
       <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
+      <c r="AG12" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AL12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1" t="s">
         <v>86</v>
@@ -2098,14 +2102,12 @@
         <v>84</v>
       </c>
       <c r="AS12" s="1"/>
-      <c r="AT12" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="AT12" s="1"/>
       <c r="AU12" s="1" t="s">
         <v>99</v>
       </c>
       <c r="AV12" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
@@ -2118,14 +2120,16 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>54</v>
@@ -2134,44 +2138,42 @@
         <v>80</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="O13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="R13" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="T13" s="1"/>
       <c r="U13" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>98</v>
@@ -2183,30 +2185,30 @@
       <c r="AA13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="AE13" s="1" t="s">
         <v>100</v>
       </c>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
+      <c r="AH13" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="AI13" s="1" t="s">
         <v>98</v>
       </c>
       <c r="AJ13" s="1"/>
-      <c r="AK13" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="AK13" s="1"/>
       <c r="AL13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM13" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1" t="s">
         <v>86</v>
@@ -2214,7 +2216,9 @@
       <c r="AP13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AQ13" s="1"/>
+      <c r="AQ13" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AR13" s="1" t="s">
         <v>84</v>
       </c>
@@ -2224,11 +2228,9 @@
         <v>100</v>
       </c>
       <c r="AV13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AW13" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
       <c r="AY13" s="1"/>
       <c r="AZ13" s="1"/>
@@ -2238,15 +2240,13 @@
       <c r="A14" s="3">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>61</v>
@@ -2255,73 +2255,77 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="L14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X14" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="Y14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AB14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AC14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="AE14" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI14" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AM14" s="1"/>
+      <c r="AM14" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1" t="s">
         <v>92</v>
@@ -2336,16 +2340,16 @@
       <c r="AS14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT14" s="1"/>
+      <c r="AT14" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="AU14" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AV14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW14" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="AW14" s="1"/>
       <c r="AX14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2357,92 +2361,96 @@
       <c r="A15" s="3">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
         <v>68</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1" t="s">
+      <c r="N15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T15" s="1"/>
+      <c r="T15" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="U15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y15" s="1"/>
       <c r="Z15" s="1" t="s">
         <v>69</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="AB15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC15" s="1"/>
       <c r="AD15" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI15" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="AJ15" s="1" t="s">
         <v>77</v>
       </c>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM15" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="AM15" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AN15" s="1" t="s">
         <v>79</v>
       </c>
@@ -2456,18 +2464,16 @@
       <c r="AR15" s="1"/>
       <c r="AS15" s="1"/>
       <c r="AT15" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="AU15" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AV15" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="AW15" s="1"/>
-      <c r="AX15" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="AX15" s="1"/>
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
@@ -2490,17 +2496,15 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
@@ -2518,9 +2522,7 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
-      <c r="AL16" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
@@ -2541,17 +2543,17 @@
       <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
         <v>104</v>
@@ -2561,75 +2563,75 @@
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
         <v>90</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="Q18" s="1"/>
       <c r="R18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="X18" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="AA18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AE18" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
+      <c r="AG18" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AM18" s="1" t="s">
         <v>74</v>
       </c>
@@ -2638,16 +2640,16 @@
         <v>104</v>
       </c>
       <c r="AP18" s="1"/>
-      <c r="AQ18" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="AQ18" s="1"/>
       <c r="AR18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AS18" s="1"/>
+      <c r="AS18" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
@@ -2663,113 +2665,117 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="J19" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L19" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="W19" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y19" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="Y19" s="1"/>
       <c r="Z19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AE19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AG19" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AJ19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL19" s="1"/>
-      <c r="AM19" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="AN19" s="1"/>
-      <c r="AO19" s="1"/>
+      <c r="AO19" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="AP19" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="AQ19" s="1"/>
       <c r="AR19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AS19" s="1"/>
+      <c r="AS19" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="AT19" s="1"/>
-      <c r="AU19" s="1"/>
-      <c r="AV19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AW19" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="AU19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
       <c r="AX19" s="1" t="s">
         <v>54</v>
       </c>
@@ -2782,112 +2788,112 @@
         <v>3</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>56</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S20" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T20" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Y20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC20" s="1" t="s">
+      <c r="AF20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG20" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AJ20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK20" s="1"/>
-      <c r="AL20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AM20" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
       <c r="AP20" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AQ20" s="1"/>
-      <c r="AR20" s="1"/>
+      <c r="AR20" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="AS20" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
-      <c r="AV20" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="AV20" s="1"/>
       <c r="AW20" s="1" t="s">
         <v>87</v>
       </c>
@@ -2904,20 +2910,20 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>56</v>
@@ -2931,91 +2937,89 @@
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O21" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="Q21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>103</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
       <c r="W21" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>109</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="AC21" s="1"/>
       <c r="AD21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE21" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="AF21" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AJ21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL21" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
-      <c r="AO21" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="AO21" s="1"/>
       <c r="AP21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ21" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="AR21" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="AS21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AT21" s="1"/>
-      <c r="AU21" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="AT21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU21" s="1"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AX21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY21" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
       <c r="AZ21" s="1"/>
       <c r="BA21" s="1"/>
     </row>
@@ -3031,22 +3035,22 @@
         <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J22" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="K22" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
@@ -3055,38 +3059,42 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
+      <c r="U22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="W22" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC22" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="AD22" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AE22" s="1" t="s">
         <v>112</v>
@@ -3097,17 +3105,19 @@
       <c r="AG22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH22" s="1"/>
+      <c r="AH22" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="AI22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ22" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="AK22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AL22" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1" t="s">
@@ -3117,15 +3127,11 @@
         <v>92</v>
       </c>
       <c r="AQ22" s="1"/>
-      <c r="AR22" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AR22" s="1"/>
       <c r="AS22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AT22" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="AT22" s="1"/>
       <c r="AU22" s="1"/>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1" t="s">
@@ -3145,114 +3151,112 @@
         <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="S23" s="1"/>
       <c r="T23" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y23" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="Z23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ23" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AK23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL23" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AL23" s="1"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AP23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AQ23" s="1"/>
-      <c r="AR23" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AR23" s="1"/>
       <c r="AS23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AT23" s="1"/>
       <c r="AU23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AV23" s="1"/>
-      <c r="AW23" s="1"/>
-      <c r="AX23" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="AV23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX23" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="AY23" s="1"/>
       <c r="AZ23" s="1"/>
       <c r="BA23" s="1"/>
@@ -3262,98 +3266,98 @@
         <v>7</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>114</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
       <c r="W24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AC24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD24" s="1" t="s">
+      <c r="AA24" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="AK24" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AQ24" s="1"/>
-      <c r="AR24" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="AQ24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR24" s="1"/>
       <c r="AS24" s="1"/>
       <c r="AT24" s="1" t="s">
         <v>90</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV24" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="AV24" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="AW24" s="1"/>
-      <c r="AX24" s="1"/>
+      <c r="AX24" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="AY24" s="1"/>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
@@ -3366,9 +3370,11 @@
         <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>80</v>
       </c>
@@ -3384,10 +3390,10 @@
         <v>60</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1" t="s">
@@ -3397,17 +3403,19 @@
         <v>52</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q26" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -3420,32 +3428,28 @@
       <c r="AA26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AE26" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AF26" s="1"/>
       <c r="AG26" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AJ26" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="AJ26" s="1"/>
       <c r="AK26" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AL26" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AM26" s="1" t="s">
         <v>74</v>
@@ -3456,17 +3460,17 @@
       </c>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="AR26" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AS26" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AV26" s="1" t="s">
         <v>91</v>
@@ -3487,15 +3491,13 @@
         <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
@@ -3507,71 +3509,69 @@
       <c r="K27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="N27" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="O27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q27" s="1"/>
       <c r="R27" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA27" s="1" t="s">
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI27" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="AG27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI27" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AL27" s="1"/>
+      <c r="AL27" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="AM27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
@@ -3579,9 +3579,11 @@
         <v>84</v>
       </c>
       <c r="AS27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AT27" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="AT27" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AU27" s="1"/>
       <c r="AV27" s="1" t="s">
         <v>91</v>
@@ -3592,7 +3594,9 @@
       <c r="AX27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AY27" s="1"/>
+      <c r="AY27" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
     </row>
@@ -3600,68 +3604,70 @@
       <c r="A28" s="3">
         <v>3</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q28" s="1"/>
       <c r="R28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-      <c r="W28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
       <c r="Y28" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Z28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AA28" s="1"/>
+      <c r="AA28" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="AB28" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1" t="s">
@@ -3671,34 +3677,30 @@
         <v>61</v>
       </c>
       <c r="AH28" s="1"/>
-      <c r="AI28" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="AI28" s="1"/>
       <c r="AJ28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK28" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="AK28" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="AL28" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AM28" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR28" s="1"/>
-      <c r="AS28" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AT28" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="AR28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
       <c r="AU28" s="1" t="s">
         <v>121</v>
       </c>
@@ -3719,7 +3721,7 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>53</v>
@@ -3727,61 +3729,59 @@
       <c r="E29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="M29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
-      <c r="X29" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="X29" s="1"/>
       <c r="Y29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Z29" s="1"/>
+      <c r="Z29" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="AA29" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AB29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
+      <c r="AC29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="AE29" s="1"/>
       <c r="AF29" s="1" t="s">
         <v>122</v>
@@ -3789,43 +3789,45 @@
       <c r="AG29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI29" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
       <c r="AJ29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK29" s="1"/>
-      <c r="AL29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM29" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="AK29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AN29" s="1"/>
-      <c r="AO29" s="1"/>
-      <c r="AP29" s="1"/>
-      <c r="AQ29" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AO29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ29" s="1"/>
       <c r="AR29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AS29" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="AS29" s="1"/>
       <c r="AT29" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AU29" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AV29" s="1"/>
+      <c r="AV29" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AW29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AX29" s="1"/>
+      <c r="AX29" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="AY29" s="1"/>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
@@ -3837,101 +3839,105 @@
       <c r="B30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N30" s="1" t="s">
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
+      <c r="Y30" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="Z30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA30" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="AA30" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="AB30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="AC30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
-      <c r="AF30" s="1"/>
-      <c r="AG30" s="1"/>
+      <c r="AF30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="AH30" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AK30" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
       <c r="AM30" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN30" s="1"/>
-      <c r="AO30" s="1"/>
-      <c r="AP30" s="1"/>
-      <c r="AQ30" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ30" s="1"/>
       <c r="AR30" s="1" t="s">
         <v>69</v>
       </c>
       <c r="AS30" s="1"/>
       <c r="AT30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU30" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="AU30" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="AV30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AW30" s="1" t="s">
         <v>87</v>
@@ -3951,106 +3957,102 @@
         <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1" t="s">
+      <c r="O31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S31" s="1"/>
+      <c r="S31" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="T31" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>69</v>
       </c>
       <c r="AA31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AB31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
-      <c r="AF31" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="AF31" s="1"/>
       <c r="AG31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH31" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AK31" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL31" s="1"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="AM31" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AN31" s="1"/>
-      <c r="AO31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP31" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
       <c r="AQ31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AR31" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="AR31" s="1"/>
       <c r="AS31" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AT31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AU31" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
       <c r="AX31" s="1" t="s">
@@ -4066,14 +4068,12 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -4082,24 +4082,26 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N32" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
         <v>58</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1" t="s">
@@ -4112,43 +4114,45 @@
       <c r="Y32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Z32" s="1"/>
+      <c r="Z32" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="AA32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD32" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="AB32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
       <c r="AG32" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="AH32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AK32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL32" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="AL32" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AM32" s="1"/>
       <c r="AN32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AO32" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP32" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="AO32" s="1"/>
+      <c r="AP32" s="1"/>
       <c r="AQ32" s="1" t="s">
         <v>69</v>
       </c>
@@ -4157,16 +4161,12 @@
         <v>84</v>
       </c>
       <c r="AT32" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="AU32" s="1"/>
-      <c r="AV32" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
-      <c r="AX32" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="AX32" s="1"/>
       <c r="AY32" s="1"/>
       <c r="AZ32" s="1"/>
       <c r="BA32" s="1"/>
@@ -4181,10 +4181,10 @@
       <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -4192,17 +4192,15 @@
         <v>56</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M34" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="M34" s="1"/>
       <c r="N34" s="1" t="s">
         <v>63</v>
       </c>
@@ -4210,9 +4208,11 @@
         <v>52</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q34" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1" t="s">
         <v>59</v>
@@ -4223,17 +4223,21 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="X34" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="Y34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z34" s="1" t="s">
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
+      <c r="AB34" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AC34" s="1" t="s">
         <v>76</v>
       </c>
@@ -4250,25 +4254,23 @@
       <c r="AJ34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AK34" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
       <c r="AM34" s="1" t="s">
         <v>74</v>
       </c>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AP34" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AQ34" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AR34" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AS34" s="1"/>
       <c r="AT34" s="1"/>
@@ -4276,9 +4278,7 @@
       <c r="AV34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AW34" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="AW34" s="1"/>
       <c r="AX34" s="1" t="s">
         <v>54</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>69</v>
@@ -4301,61 +4301,59 @@
         <v>79</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="J35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="R35" s="1"/>
       <c r="S35" s="1" t="s">
         <v>73</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="X35" s="1"/>
+      <c r="X35" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="Y35" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="Z35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AA35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB35" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AB35" s="1"/>
       <c r="AC35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AD35" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
@@ -4365,14 +4363,16 @@
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK35" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="AK35" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="AL35" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AM35" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
@@ -4380,10 +4380,10 @@
       <c r="AQ35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AR35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS35" s="1"/>
+      <c r="AR35" s="1"/>
+      <c r="AS35" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="AT35" s="1"/>
       <c r="AU35" s="1"/>
       <c r="AV35" s="1" t="s">
@@ -4407,9 +4407,7 @@
         <v>78</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>79</v>
       </c>
@@ -4420,19 +4418,19 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="N36" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>52</v>
@@ -4441,9 +4439,11 @@
         <v>56</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R36" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1" t="s">
         <v>65</v>
@@ -4457,46 +4457,46 @@
       <c r="Y36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Z36" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="Z36" s="1"/>
       <c r="AA36" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AB36" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="AC36" s="1"/>
-      <c r="AD36" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
       <c r="AF36" s="1"/>
       <c r="AG36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH36" s="1"/>
+      <c r="AH36" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="AI36" s="1"/>
-      <c r="AJ36" s="1"/>
-      <c r="AK36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL36" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="AJ36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
       <c r="AM36" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
-      <c r="AQ36" s="1"/>
+      <c r="AQ36" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="AR36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AS36" s="1"/>
+      <c r="AS36" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="AT36" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="AU36" s="1"/>
       <c r="AV36" s="1" t="s">
@@ -4533,47 +4533,47 @@
       <c r="H37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="Q37" s="1"/>
       <c r="R37" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T37" s="1"/>
+      <c r="T37" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
+      <c r="W37" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="X37" s="1"/>
-      <c r="Y37" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
+      <c r="AA37" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="AB37" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="AC37" s="1" t="s">
         <v>84</v>
@@ -4587,25 +4587,25 @@
         <v>61</v>
       </c>
       <c r="AH37" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI37" s="1"/>
-      <c r="AJ37" s="1"/>
-      <c r="AK37" s="1"/>
+      <c r="AJ37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK37" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="AL37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AM37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AN37" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
       <c r="AP37" s="1"/>
-      <c r="AQ37" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="AQ37" s="1"/>
       <c r="AR37" s="1" t="s">
         <v>69</v>
       </c>
@@ -4629,55 +4629,51 @@
       <c r="A38" s="3">
         <v>5</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F38" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="J38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q38" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="R38" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T38" s="1"/>
+      <c r="T38" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1" t="s">
@@ -4685,10 +4681,10 @@
       </c>
       <c r="X38" s="1"/>
       <c r="Y38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1" t="s">
@@ -4697,39 +4693,43 @@
       <c r="AC38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AD38" s="1"/>
+      <c r="AD38" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="AE38" s="1"/>
       <c r="AF38" s="1"/>
-      <c r="AG38" s="1"/>
-      <c r="AH38" s="1" t="s">
+      <c r="AG38" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK38" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="AK38" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="AL38" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AM38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN38" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="AN38" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AO38" s="1"/>
       <c r="AP38" s="1"/>
-      <c r="AQ38" s="1"/>
-      <c r="AR38" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AQ38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR38" s="1"/>
       <c r="AS38" s="1"/>
       <c r="AT38" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AU38" s="1"/>
-      <c r="AV38" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="AV38" s="1"/>
       <c r="AW38" s="1" t="s">
         <v>87</v>
       </c>
@@ -4742,108 +4742,108 @@
       <c r="A39" s="3">
         <v>6</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
+      <c r="J39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="L39" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N39" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T39" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA39" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="AA39" s="1"/>
       <c r="AB39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="AD39" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="AE39" s="1"/>
       <c r="AF39" s="1"/>
-      <c r="AG39" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="AG39" s="1"/>
       <c r="AH39" s="1" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="AI39" s="1"/>
-      <c r="AJ39" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="AJ39" s="1"/>
       <c r="AK39" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AL39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AM39" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM39" s="1"/>
       <c r="AN39" s="1" t="s">
         <v>91</v>
       </c>
       <c r="AO39" s="1"/>
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR39" s="1"/>
-      <c r="AS39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR39" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="AS39" s="1"/>
       <c r="AT39" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="AU39" s="1"/>
-      <c r="AV39" s="1"/>
-      <c r="AW39" s="1"/>
+      <c r="AV39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW39" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="AX39" s="1"/>
       <c r="AY39" s="1" t="s">
         <v>78</v>
@@ -4875,42 +4875,40 @@
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>78</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>57</v>
       </c>
       <c r="S40" s="1"/>
-      <c r="T40" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1" t="s">
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z40" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="AA40" s="1"/>
       <c r="AB40" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="AC40" s="1" t="s">
         <v>68</v>
@@ -4930,12 +4928,14 @@
         <v>69</v>
       </c>
       <c r="AJ40" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="AK40" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL40" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="AL40" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="AM40" s="1"/>
       <c r="AN40" s="1" t="s">
         <v>91</v>
@@ -4945,16 +4945,16 @@
       <c r="AQ40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AR40" s="1"/>
-      <c r="AS40" s="1" t="s">
+      <c r="AR40" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="AS40" s="1"/>
       <c r="AT40" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AU40" s="1"/>
       <c r="AV40" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AW40" s="1"/>
       <c r="AX40" s="1" t="s">

</xml_diff>